<commit_message>
update teams info and collect data
</commit_message>
<xml_diff>
--- a/submissions/teams_overview.xlsx
+++ b/submissions/teams_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raoulcollenteur/Github/gwm_challenge/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA811CAA-AB7F-6A4C-95C8-617C8D085B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00681F7C-C789-FD47-A0D5-5E84D0511B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{73C169F9-F963-4543-90A2-22E8DBE5135E}"/>
+    <workbookView xWindow="-38380" yWindow="-1980" windowWidth="38380" windowHeight="21100" xr2:uid="{73C169F9-F963-4543-90A2-22E8DBE5135E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="52">
   <si>
     <t>Team</t>
   </si>
@@ -170,9 +170,6 @@
     <t>HydroSight</t>
   </si>
   <si>
-    <t>Time information</t>
-  </si>
-  <si>
     <t>General Info</t>
   </si>
   <si>
@@ -189,6 +186,12 @@
   </si>
   <si>
     <t>Shallow learners Ensemble</t>
+  </si>
+  <si>
+    <t>Development time</t>
+  </si>
+  <si>
+    <t>Calibration time</t>
   </si>
 </sst>
 </file>
@@ -227,7 +230,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -264,26 +267,126 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EE707B4-2C95-AD48-8C53-62E67E7F1874}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,29 +716,46 @@
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="D1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="10"/>
       <c r="I1" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="10"/>
+    </row>
+    <row r="2" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -653,430 +773,945 @@
       <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
+      <c r="D3" s="13">
+        <v>1</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+      <c r="G3" s="13">
         <v>1</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I3" s="22">
+        <v>4</v>
+      </c>
+      <c r="J3" s="23">
+        <v>4</v>
+      </c>
+      <c r="K3" s="23">
+        <v>4</v>
+      </c>
+      <c r="L3" s="23">
+        <v>4</v>
+      </c>
+      <c r="M3" s="24">
+        <v>4</v>
+      </c>
+      <c r="N3" s="22">
+        <v>2</v>
+      </c>
+      <c r="O3" s="23">
+        <v>2</v>
+      </c>
+      <c r="P3" s="23">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>2</v>
+      </c>
+      <c r="R3" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="13">
         <v>1</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I4" s="22">
+        <v>2</v>
+      </c>
+      <c r="J4" s="23">
+        <v>2</v>
+      </c>
+      <c r="K4" s="23">
+        <v>2</v>
+      </c>
+      <c r="L4" s="23">
+        <v>2</v>
+      </c>
+      <c r="M4" s="24">
+        <v>2</v>
+      </c>
+      <c r="N4" s="22">
+        <v>15</v>
+      </c>
+      <c r="O4" s="22">
+        <v>15</v>
+      </c>
+      <c r="P4" s="22">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="22">
+        <v>15</v>
+      </c>
+      <c r="R4" s="22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1</v>
+      </c>
+      <c r="G5" s="13">
         <v>1</v>
       </c>
       <c r="H5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I5" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="J5" s="25">
+        <v>5</v>
+      </c>
+      <c r="K5" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="24">
+        <v>1</v>
+      </c>
+      <c r="N5" s="22">
+        <f>345/60/60</f>
+        <v>9.583333333333334E-2</v>
+      </c>
+      <c r="O5" s="25">
+        <f>310/60/60</f>
+        <v>8.611111111111111E-2</v>
+      </c>
+      <c r="P5" s="25">
+        <f>48/60/60</f>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="Q5" s="25">
+        <f>60/60/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="R5" s="24">
+        <f>289/60/60</f>
+        <v>8.0277777777777767E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
+      <c r="C6" s="12"/>
+      <c r="D6" s="13">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1</v>
+      </c>
+      <c r="G6" s="13">
         <v>1</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I6" s="22">
+        <v>4</v>
+      </c>
+      <c r="J6" s="25">
+        <v>4</v>
+      </c>
+      <c r="K6" s="25">
+        <v>4</v>
+      </c>
+      <c r="L6" s="25">
+        <v>4</v>
+      </c>
+      <c r="M6" s="24">
+        <v>4</v>
+      </c>
+      <c r="N6" s="22">
+        <v>2</v>
+      </c>
+      <c r="O6" s="25">
+        <v>2</v>
+      </c>
+      <c r="P6" s="25">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="25">
+        <v>2</v>
+      </c>
+      <c r="R6" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
+      <c r="C7" s="12"/>
+      <c r="D7" s="13">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1</v>
+      </c>
+      <c r="G7" s="13">
         <v>1</v>
       </c>
       <c r="H7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I7" s="22">
+        <v>5</v>
+      </c>
+      <c r="J7" s="25">
+        <v>5</v>
+      </c>
+      <c r="K7" s="25">
+        <v>5</v>
+      </c>
+      <c r="L7" s="25">
+        <v>5</v>
+      </c>
+      <c r="M7" s="24">
+        <v>5</v>
+      </c>
+      <c r="N7" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="O7" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="P7" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="Q7" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="R7" s="22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
+      <c r="D8" s="13">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
         <v>1</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I8" s="22">
+        <v>3</v>
+      </c>
+      <c r="J8" s="25">
+        <v>3</v>
+      </c>
+      <c r="K8" s="25">
+        <v>3</v>
+      </c>
+      <c r="L8" s="25">
+        <v>3</v>
+      </c>
+      <c r="M8" s="24">
+        <v>3</v>
+      </c>
+      <c r="N8" s="22">
+        <f>5570/60/60</f>
+        <v>1.5472222222222221</v>
+      </c>
+      <c r="O8" s="25">
+        <f>(150+4680)/60/60</f>
+        <v>1.3416666666666666</v>
+      </c>
+      <c r="P8" s="25">
+        <f>(20+1800)/60/60</f>
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="Q8" s="25">
+        <f>(20+1800)/60/60</f>
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="R8" s="25">
+        <f>(80+1800)/60/60</f>
+        <v>0.52222222222222225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="13">
         <v>0</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="13">
         <v>0</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
+      <c r="F9" s="13">
+        <v>1</v>
+      </c>
+      <c r="G9" s="13">
         <v>0</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I9" s="22"/>
+      <c r="J9" s="25">
+        <v>4</v>
+      </c>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="25">
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="24"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10">
+      <c r="C10" s="12"/>
+      <c r="D10" s="13">
         <v>0</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
         <v>0</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I10" s="22">
+        <v>4</v>
+      </c>
+      <c r="J10" s="25">
+        <v>30</v>
+      </c>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="22">
+        <f>140/60/60</f>
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="O10" s="25">
+        <f>168/60/60</f>
+        <v>4.6666666666666662E-2</v>
+      </c>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="24"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
+      <c r="D11" s="13">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13">
         <v>0</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="13">
         <v>0</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I11" s="22">
+        <v>4</v>
+      </c>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="N11" s="22">
+        <v>48</v>
+      </c>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="24">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
+      <c r="C12" s="12"/>
+      <c r="D12" s="13">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13">
+        <v>1</v>
+      </c>
+      <c r="G12" s="13">
         <v>1</v>
       </c>
       <c r="H12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I12" s="22">
+        <v>3</v>
+      </c>
+      <c r="J12" s="25">
+        <v>3</v>
+      </c>
+      <c r="K12" s="25">
+        <v>1</v>
+      </c>
+      <c r="L12" s="25">
+        <v>1</v>
+      </c>
+      <c r="M12" s="24">
+        <v>3</v>
+      </c>
+      <c r="N12" s="22"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="24"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13">
         <v>1</v>
       </c>
       <c r="H13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I13" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="J13" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="K13" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="L13" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M13" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="N13" s="22">
+        <f>40/60/60</f>
+        <v>1.111111111111111E-2</v>
+      </c>
+      <c r="O13" s="22">
+        <f>40/60/60</f>
+        <v>1.111111111111111E-2</v>
+      </c>
+      <c r="P13" s="22">
+        <f>40/60/60</f>
+        <v>1.111111111111111E-2</v>
+      </c>
+      <c r="Q13" s="22">
+        <f>40/60/60</f>
+        <v>1.111111111111111E-2</v>
+      </c>
+      <c r="R13" s="22">
+        <f>40/60/60</f>
+        <v>1.111111111111111E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13">
         <v>1</v>
       </c>
       <c r="H14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I14" s="22">
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J14" s="22">
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K14" s="22">
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="L14" s="22">
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M14" s="22">
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="N14" s="22">
+        <v>2</v>
+      </c>
+      <c r="O14" s="25">
+        <v>2</v>
+      </c>
+      <c r="P14" s="25">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="25">
+        <v>2</v>
+      </c>
+      <c r="R14" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
+      <c r="C15" s="12"/>
+      <c r="D15" s="13">
+        <v>1</v>
+      </c>
+      <c r="E15" s="13">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13">
+        <v>1</v>
+      </c>
+      <c r="G15" s="13">
         <v>1</v>
       </c>
       <c r="H15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I15" s="22">
+        <v>4</v>
+      </c>
+      <c r="J15" s="25">
+        <v>4</v>
+      </c>
+      <c r="K15" s="25">
+        <v>4</v>
+      </c>
+      <c r="L15" s="25">
+        <v>4</v>
+      </c>
+      <c r="M15" s="24">
+        <v>4</v>
+      </c>
+      <c r="N15" s="22">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="O15" s="22">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="P15" s="22">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="Q15" s="22">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="R15" s="22">
+        <v>1.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="13">
         <v>0</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
+      <c r="E16" s="13">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13">
+        <v>1</v>
+      </c>
+      <c r="G16" s="13">
         <v>1</v>
       </c>
       <c r="H16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="22">
+        <v>2</v>
+      </c>
+      <c r="J16" s="25">
+        <v>2</v>
+      </c>
+      <c r="K16" s="25">
+        <v>2</v>
+      </c>
+      <c r="L16" s="25">
+        <v>2</v>
+      </c>
+      <c r="M16" s="24">
+        <v>2</v>
+      </c>
+      <c r="N16" s="22">
+        <f>2700/60/60</f>
+        <v>0.75</v>
+      </c>
+      <c r="O16" s="22">
+        <f>2700/60/60</f>
+        <v>0.75</v>
+      </c>
+      <c r="P16" s="22">
+        <f>2700/60/60</f>
+        <v>0.75</v>
+      </c>
+      <c r="Q16" s="22">
+        <f>2700/60/60</f>
+        <v>0.75</v>
+      </c>
+      <c r="R16" s="22">
+        <f>2700/60/60</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
+      <c r="C17" s="12"/>
+      <c r="D17" s="13">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13">
+        <v>1</v>
+      </c>
+      <c r="F17" s="13">
+        <v>1</v>
+      </c>
+      <c r="G17" s="13">
         <v>1</v>
       </c>
       <c r="H17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="22">
+        <v>2</v>
+      </c>
+      <c r="J17" s="25">
+        <v>6</v>
+      </c>
+      <c r="K17" s="25">
+        <v>3</v>
+      </c>
+      <c r="L17" s="25">
+        <v>2</v>
+      </c>
+      <c r="M17" s="24">
+        <v>2</v>
+      </c>
+      <c r="N17" s="22">
+        <f>600/60/60</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="O17" s="22">
+        <f>600/60/60</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P17" s="22">
+        <f>300/60/60</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="Q17" s="22">
+        <f>300/60/60</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="R17" s="22">
+        <f>600/60/60</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
+      <c r="D18" s="13">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13">
+        <v>1</v>
+      </c>
+      <c r="G18" s="13">
         <v>1</v>
       </c>
       <c r="H18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="22">
+        <v>2</v>
+      </c>
+      <c r="J18" s="23">
+        <v>2</v>
+      </c>
+      <c r="K18" s="23">
+        <v>2</v>
+      </c>
+      <c r="L18" s="23">
+        <v>2</v>
+      </c>
+      <c r="M18" s="24">
+        <v>2</v>
+      </c>
+      <c r="N18" s="22">
+        <v>2</v>
+      </c>
+      <c r="O18" s="23">
+        <v>2</v>
+      </c>
+      <c r="P18" s="23">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="23">
+        <v>2</v>
+      </c>
+      <c r="R18" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D19">
+      <c r="C19" s="14"/>
+      <c r="D19" s="15">
         <v>0</v>
       </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
+      <c r="E19" s="15">
+        <v>1</v>
+      </c>
+      <c r="F19" s="15">
+        <v>1</v>
+      </c>
+      <c r="G19" s="15">
         <v>0</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="16">
         <v>0</v>
       </c>
+      <c r="I19" s="26">
+        <v>72</v>
+      </c>
+      <c r="J19" s="27">
+        <v>72</v>
+      </c>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="26">
+        <v>5</v>
+      </c>
+      <c r="O19" s="27">
+        <v>5</v>
+      </c>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="27"/>
+      <c r="R19" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1087,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6926E848-AF46-FA41-BD7A-781BF4FEB007}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G18"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1114,13 +1749,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1133,17 +1768,17 @@
       <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>49</v>
+      <c r="D2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1156,17 +1791,17 @@
       <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>49</v>
+      <c r="D3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1179,17 +1814,17 @@
       <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>49</v>
+      <c r="D4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1199,17 +1834,17 @@
       <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>49</v>
+      <c r="D5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1219,17 +1854,17 @@
       <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>49</v>
+      <c r="D6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1242,17 +1877,17 @@
       <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>49</v>
+      <c r="D7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1265,12 +1900,12 @@
       <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="10"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1279,14 +1914,14 @@
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="10"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1298,14 +1933,14 @@
       <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
+      <c r="D10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1314,17 +1949,17 @@
       <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>49</v>
+      <c r="D11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1337,17 +1972,17 @@
       <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>49</v>
+      <c r="D12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1360,17 +1995,17 @@
       <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>49</v>
+      <c r="D13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1378,40 +2013,40 @@
         <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>49</v>
+      <c r="D14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>49</v>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1421,17 +2056,17 @@
       <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>49</v>
+      <c r="D16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1444,17 +2079,17 @@
       <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>49</v>
+      <c r="D17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1464,14 +2099,14 @@
       <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="10"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update data collection notebook
</commit_message>
<xml_diff>
--- a/submissions/teams_overview.xlsx
+++ b/submissions/teams_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clientadmin/GitHub/gmc/gmc_teams/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7250332A-F803-B943-9944-D98F8689509B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A42888-2E1D-D246-A83E-83103205CDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="500" windowWidth="38380" windowHeight="21100" xr2:uid="{73C169F9-F963-4543-90A2-22E8DBE5135E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{73C169F9-F963-4543-90A2-22E8DBE5135E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -723,7 +723,7 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -731,10 +731,10 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -750,8 +750,7 @@
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
+      <c r="G1" s="10"/>
       <c r="I1" s="8" t="s">
         <v>50</v>
       </c>
@@ -778,19 +777,19 @@
         <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>3</v>
@@ -842,10 +841,10 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" s="17">
@@ -898,10 +897,10 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" s="17">
@@ -954,10 +953,10 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
       <c r="I5" s="17">
@@ -1015,10 +1014,10 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6">
         <v>1</v>
       </c>
       <c r="I6" s="17">
@@ -1071,10 +1070,10 @@
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>1</v>
       </c>
       <c r="I7" s="17">
@@ -1127,10 +1126,10 @@
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8">
         <v>1</v>
       </c>
       <c r="I8" s="17">
@@ -1183,15 +1182,15 @@
         <v>0</v>
       </c>
       <c r="E9" s="24">
+        <v>1</v>
+      </c>
+      <c r="F9" s="24">
         <v>0</v>
       </c>
-      <c r="F9" s="24">
-        <v>1</v>
-      </c>
-      <c r="G9" s="24">
+      <c r="G9" s="27">
         <v>0</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="24">
         <v>0</v>
       </c>
       <c r="I9" s="28"/>
@@ -1221,18 +1220,18 @@
         <v>52</v>
       </c>
       <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>0</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>0</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10">
         <v>0</v>
       </c>
       <c r="I10" s="17">
@@ -1270,16 +1269,16 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="1">
-        <v>0</v>
+      <c r="H11">
+        <v>1</v>
       </c>
       <c r="I11" s="17">
         <v>4</v>
@@ -1319,10 +1318,10 @@
       <c r="F12">
         <v>1</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12">
         <v>1</v>
       </c>
       <c r="I12" s="17">
@@ -1365,10 +1364,10 @@
       <c r="F13">
         <v>1</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>1</v>
       </c>
       <c r="I13" s="17">
@@ -1426,10 +1425,10 @@
       <c r="F14">
         <v>1</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1">
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14">
         <v>1</v>
       </c>
       <c r="I14" s="17">
@@ -1476,7 +1475,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1487,10 +1486,10 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15">
         <v>1</v>
       </c>
       <c r="I15" s="17">
@@ -1535,19 +1534,19 @@
         <v>52</v>
       </c>
       <c r="D16" s="24">
+        <v>1</v>
+      </c>
+      <c r="E16" s="24">
+        <v>1</v>
+      </c>
+      <c r="F16" s="24">
+        <v>1</v>
+      </c>
+      <c r="G16" s="27">
+        <v>1</v>
+      </c>
+      <c r="H16" s="24">
         <v>0</v>
-      </c>
-      <c r="E16" s="24">
-        <v>1</v>
-      </c>
-      <c r="F16" s="24">
-        <v>1</v>
-      </c>
-      <c r="G16" s="24">
-        <v>1</v>
-      </c>
-      <c r="H16" s="27">
-        <v>1</v>
       </c>
       <c r="I16" s="28">
         <v>2</v>
@@ -1604,10 +1603,10 @@
       <c r="F17">
         <v>1</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17">
         <v>1</v>
       </c>
       <c r="I17" s="17">
@@ -1665,10 +1664,10 @@
       <c r="F18">
         <v>1</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" s="17">
@@ -1713,18 +1712,18 @@
         <v>37</v>
       </c>
       <c r="D19" s="13">
+        <v>1</v>
+      </c>
+      <c r="E19" s="13">
+        <v>1</v>
+      </c>
+      <c r="F19" s="13">
         <v>0</v>
       </c>
-      <c r="E19" s="13">
-        <v>1</v>
-      </c>
-      <c r="F19" s="13">
-        <v>1</v>
-      </c>
-      <c r="G19" s="13">
+      <c r="G19" s="14">
         <v>0</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="13">
         <v>0</v>
       </c>
       <c r="I19" s="20">

</xml_diff>